<commit_message>
add cell value change setting
</commit_message>
<xml_diff>
--- a/GBTH/bin/Debug/net6.0-windows/default.xlsx
+++ b/GBTH/bin/Debug/net6.0-windows/default.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\source\repos\elecbug\CSharp\GBTH\bin\Debug\net6.0-windows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DEE4F5-0ED5-4A7B-8927-B9C240B3C131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2CCDC8-3E37-4F1D-AEE3-5C6C5FD90F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" xr2:uid="{A60E88F6-742F-46AF-85FD-79EB5DDDF4A7}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8964" xr2:uid="{A60E88F6-742F-46AF-85FD-79EB5DDDF4A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>